<commit_message>
fix: [SK-1.0] separating contact information in lead
</commit_message>
<xml_diff>
--- a/campaignSchema.xlsx
+++ b/campaignSchema.xlsx
@@ -11,8 +11,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -43,8 +45,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,523 +392,512 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
+      <c r="A1" s="1" t="str">
         <v>_id</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" s="1" t="str">
         <v>internalField</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" s="1" t="str">
         <v>name</v>
       </c>
-      <c r="D1" t="str">
+      <c r="D1" s="1" t="str">
         <v>organization</v>
       </c>
-      <c r="E1" t="str">
+      <c r="E1" s="1" t="str">
         <v>__v</v>
       </c>
-      <c r="F1" t="str">
+      <c r="F1" s="1" t="str">
         <v>checked</v>
       </c>
-      <c r="G1" t="str">
+      <c r="G1" s="1" t="str">
         <v>readableField</v>
       </c>
-      <c r="H1" t="str">
+      <c r="H1" s="1" t="str">
         <v>type</v>
       </c>
-      <c r="I1" t="str">
-        <v>options</v>
+      <c r="I1" s="1" t="str">
+        <v>group</v>
       </c>
     </row>
     <row r="2">
-      <c r="B2" t="str">
+      <c r="B2" s="1" t="str">
         <v>_id</v>
       </c>
-      <c r="C2" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="str">
+      <c r="C2" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="str">
         <v>CRM Id</v>
       </c>
-      <c r="H2" t="str">
+      <c r="H2" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="str">
+      <c r="B3" s="1" t="str">
         <v>address</v>
       </c>
-      <c r="C3" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" t="str">
+      <c r="C3" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="str">
         <v>Address</v>
       </c>
-      <c r="H3" t="str">
+      <c r="H3" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" t="str">
+      <c r="B4" s="1" t="str">
         <v>alternateMobile</v>
       </c>
-      <c r="C4" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="str">
+      <c r="C4" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="str">
         <v>Alternate Mobile</v>
       </c>
-      <c r="H4" t="str">
+      <c r="H4" s="1" t="str">
         <v>tel</v>
       </c>
+      <c r="I4" s="1" t="str">
+        <v>contact</v>
+      </c>
     </row>
     <row r="5">
-      <c r="B5" t="str">
+      <c r="B5" s="1" t="str">
         <v>amount</v>
       </c>
-      <c r="C5" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="str">
+      <c r="C5" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="str">
         <v>Amount</v>
       </c>
-      <c r="H5" t="str">
+      <c r="H5" s="1" t="str">
         <v>number</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="str">
+      <c r="B6" s="1" t="str">
         <v>bucket</v>
       </c>
-      <c r="C6" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="str">
+      <c r="C6" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="str">
         <v>Bucket</v>
       </c>
-      <c r="H6" t="str">
+      <c r="H6" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="str">
+      <c r="B7" s="1" t="str">
         <v>disposition</v>
       </c>
-      <c r="C7" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" t="str">
+      <c r="C7" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="str">
         <v>Call Disposition</v>
       </c>
-      <c r="H7" t="str">
+      <c r="H7" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" t="str">
+      <c r="B8" s="1" t="str">
         <v>companyName</v>
       </c>
-      <c r="C8" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" t="str">
+      <c r="C8" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="str">
         <v>Company</v>
       </c>
-      <c r="H8" t="str">
+      <c r="H8" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" t="str">
+      <c r="B9" s="1" t="str">
         <v>createdAt</v>
       </c>
-      <c r="C9" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" t="str">
+      <c r="C9" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="str">
         <v>Created At</v>
       </c>
-      <c r="H9" t="str">
+      <c r="H9" s="1" t="str">
         <v>date</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" t="str">
+      <c r="B10" s="1" t="str">
         <v>customerEmail</v>
       </c>
-      <c r="C10" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" t="str">
+      <c r="C10" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="str">
         <v>Customer Email</v>
       </c>
-      <c r="H10" t="str">
-        <v>string</v>
+      <c r="H10" s="1" t="str">
+        <v>string</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <v>contact</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" t="str">
+      <c r="B11" s="1" t="str">
         <v>email</v>
       </c>
-      <c r="C11" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" t="str">
+      <c r="C11" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="str">
         <v>Email Id</v>
       </c>
-      <c r="H11" t="str">
+      <c r="H11" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" t="str">
+      <c r="B12" s="1" t="str">
         <v>externalId</v>
       </c>
-      <c r="C12" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" t="str">
+      <c r="C12" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="str">
         <v>Lead Id</v>
       </c>
-      <c r="H12" t="str">
+      <c r="H12" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" t="str">
+      <c r="B13" s="1" t="str">
         <v>firstName</v>
       </c>
-      <c r="C13" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" t="str">
+      <c r="C13" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="str">
         <v>First Name</v>
       </c>
-      <c r="H13" t="str">
+      <c r="H13" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" t="str">
+      <c r="B14" s="1" t="str">
         <v>followUp</v>
       </c>
-      <c r="C14" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" t="str">
+      <c r="C14" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="str">
         <v>Follow Up</v>
       </c>
-      <c r="H14" t="str">
+      <c r="H14" s="1" t="str">
         <v>date</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" t="str">
+      <c r="B15" s="1" t="str">
         <v>geoLocation</v>
       </c>
-      <c r="C15" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" t="str">
+      <c r="C15" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="str">
         <v>Geo Location</v>
       </c>
-      <c r="H15" t="str">
+      <c r="H15" s="1" t="str">
         <v>geo</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" t="str">
+      <c r="B16" s="1" t="str">
         <v>lastName</v>
       </c>
-      <c r="C16" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" t="str">
+      <c r="C16" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="str">
         <v>Last Name</v>
       </c>
-      <c r="H16" t="str">
+      <c r="H16" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" t="str">
+      <c r="B17" s="1" t="str">
         <v>leadStatus</v>
       </c>
-      <c r="C17" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" t="str">
+      <c r="C17" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="str">
         <v>Lead Status</v>
       </c>
-      <c r="H17" t="str">
-        <v>select</v>
+      <c r="H17" s="1" t="str">
+        <v>string</v>
       </c>
     </row>
     <row r="18">
-      <c r="B18" t="str">
+      <c r="B18" s="1" t="str">
         <v>operationalArea</v>
       </c>
-      <c r="C18" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" t="str">
+      <c r="C18" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="str">
         <v>Operational Area</v>
       </c>
-      <c r="H18" t="str">
+      <c r="H18" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="19">
-      <c r="B19" t="str">
+      <c r="B19" s="1" t="str">
         <v>phoneNumber</v>
       </c>
-      <c r="C19" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" t="str">
-        <v>Phone Number</v>
-      </c>
-      <c r="H19" t="str">
+      <c r="C19" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <v>Mobile Number</v>
+      </c>
+      <c r="H19" s="1" t="str">
         <v>tel</v>
       </c>
+      <c r="I19" s="1" t="str">
+        <v>contact</v>
+      </c>
     </row>
     <row r="20">
-      <c r="B20" t="str">
+      <c r="B20" s="1" t="str">
         <v>phoneNumberPrefix</v>
       </c>
-      <c r="C20" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" t="str">
+      <c r="C20" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="str">
         <v>Country Code</v>
       </c>
-      <c r="H20" t="str">
+      <c r="H20" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" t="str">
+      <c r="B21" s="1" t="str">
         <v>pinCode</v>
       </c>
-      <c r="C21" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="str">
+      <c r="C21" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1" t="str">
         <v>Pin Code</v>
       </c>
-      <c r="H21" t="str">
+      <c r="H21" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" t="str">
-        <v>product</v>
-      </c>
-      <c r="C22" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22" t="str">
-        <v>Product</v>
-      </c>
-      <c r="H22" t="str">
+      <c r="B22" s="1" t="str">
+        <v>remarks</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <v>Remarks</v>
+      </c>
+      <c r="H22" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" t="str">
-        <v>remarks</v>
-      </c>
-      <c r="C23" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23" t="b">
-        <v>0</v>
-      </c>
-      <c r="G23" t="str">
-        <v>Remarks</v>
-      </c>
-      <c r="H23" t="str">
+      <c r="B23" s="1" t="str">
+        <v>source</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <v>Source</v>
+      </c>
+      <c r="H23" s="1" t="str">
         <v>string</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" t="str">
-        <v>source</v>
-      </c>
-      <c r="C24" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" t="str">
-        <v>Source</v>
-      </c>
-      <c r="H24" t="str">
-        <v>string</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="str">
+      <c r="B24" s="1" t="str">
         <v>updatedAt</v>
       </c>
-      <c r="C25" t="str">
-        <v>Mobile-v1</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G25" t="str">
+      <c r="C24" s="1" t="str">
+        <v>Mobile-v1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1" t="str">
         <v>Updated At</v>
       </c>
-      <c r="H25" t="str">
+      <c r="H24" s="1" t="str">
         <v>date</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I24"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>